<commit_message>
configured REFramework to use Browser variables and DataRow transaction items
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\P3\uipath-automation-1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0C4C16-19A7-4FCA-B851-2761B1508B3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9389375-7AFB-4DAD-9164-9F4E916635D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25875" yWindow="2175" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2004" yWindow="756" windowWidth="17280" windowHeight="8976" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
@@ -146,6 +146,18 @@
   </si>
   <si>
     <t>Credential used to sign into the Zoho account</t>
+  </si>
+  <si>
+    <t>Status_Success</t>
+  </si>
+  <si>
+    <t>Status_Failed</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Failed</t>
   </si>
 </sst>
 </file>
@@ -523,7 +535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1636,7 +1648,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -1761,8 +1775,22 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
added email input file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\P3\uipath-automation-1\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ohhey\Desktop\Revature_Workspace\uipath-automation-1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9389375-7AFB-4DAD-9164-9F4E916635D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9608A20-3CEF-4ECB-A737-EF45969BDB2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2004" yWindow="756" windowWidth="17280" windowHeight="8976" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -158,6 +158,15 @@
   </si>
   <si>
     <t>Failed</t>
+  </si>
+  <si>
+    <t>EmailWorkbookPath</t>
+  </si>
+  <si>
+    <t>Data\Input\AssociateEmails</t>
+  </si>
+  <si>
+    <t>workbook containing associate emails</t>
   </si>
 </sst>
 </file>
@@ -535,16 +544,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5234375" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.41796875" customWidth="1"/>
+    <col min="4" max="26" width="8.68359375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -629,7 +638,17 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
@@ -1648,16 +1667,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.41796875" customWidth="1"/>
+    <col min="4" max="26" width="8.68359375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2778,12 +2797,12 @@
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.89453125" customWidth="1"/>
+    <col min="2" max="2" width="30.1015625" customWidth="1"/>
+    <col min="3" max="3" width="60.3125" customWidth="1"/>
+    <col min="4" max="26" width="65.41796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Fixed dispatcher to user only 1 browser
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ohhey\Desktop\Revature_Workspace\uipath-automation-1\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\201019-UTA0UiPath\uipath-automation-1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9608A20-3CEF-4ECB-A737-EF45969BDB2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995293F3-64D2-42CF-B99C-A1C6B8C31F4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4305" yWindow="3720" windowWidth="28800" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -163,10 +163,10 @@
     <t>EmailWorkbookPath</t>
   </si>
   <si>
-    <t>Data\Input\AssociateEmails</t>
-  </si>
-  <si>
     <t>workbook containing associate emails</t>
+  </si>
+  <si>
+    <t>Data\Input\AssociateEmails.xlsx</t>
   </si>
 </sst>
 </file>
@@ -545,15 +545,15 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5234375" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.41796875" customWidth="1"/>
-    <col min="4" max="26" width="8.68359375" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -602,7 +602,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="28.8">
+    <row r="4" spans="1:26" ht="30">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -643,10 +643,10 @@
         <v>44</v>
       </c>
       <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
         <v>45</v>
-      </c>
-      <c r="C10" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1671,12 +1671,12 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.41796875" customWidth="1"/>
-    <col min="4" max="26" width="8.68359375" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1713,7 +1713,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2797,12 +2797,12 @@
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.89453125" customWidth="1"/>
-    <col min="2" max="2" width="30.1015625" customWidth="1"/>
-    <col min="3" max="3" width="60.3125" customWidth="1"/>
-    <col min="4" max="26" width="65.41796875" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Refactored code to make better use of Config constant, made Process more extensible
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\201019-UTA0UiPath\uipath-automation-1\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\P3\uipath-automation-1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC10A72-CBCD-4A3F-B42B-7D2F8162039D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FEF7499-147E-4760-BCBE-BCB094D5FEF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4305" yWindow="3720" windowWidth="28800" windowHeight="15420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -151,9 +151,6 @@
     <t>Status_Success</t>
   </si>
   <si>
-    <t>Status_Failed</t>
-  </si>
-  <si>
     <t>Success</t>
   </si>
   <si>
@@ -176,6 +173,27 @@
   </si>
   <si>
     <t>Prompt used in email body before the Google Form link</t>
+  </si>
+  <si>
+    <t>EmailService_Zoho</t>
+  </si>
+  <si>
+    <t>Gmail</t>
+  </si>
+  <si>
+    <t>Zoho</t>
+  </si>
+  <si>
+    <t>EmailService_Gmail</t>
+  </si>
+  <si>
+    <t>Status_Pending</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Status_Failure</t>
   </si>
 </sst>
 </file>
@@ -557,12 +575,12 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -611,7 +629,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="30">
+    <row r="4" spans="1:26" ht="28.8">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -649,13 +667,13 @@
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
         <v>44</v>
-      </c>
-      <c r="B10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1674,18 +1692,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z987"/>
+  <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1722,7 +1740,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1808,45 +1826,66 @@
         <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" t="s">
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
         <v>47</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C17" t="s">
         <v>48</v>
       </c>
-      <c r="C16" t="s">
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
         <v>49</v>
       </c>
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -2802,6 +2841,7 @@
     <row r="985" ht="14.25" customHeight="1"/>
     <row r="986" ht="14.25" customHeight="1"/>
     <row r="987" ht="14.25" customHeight="1"/>
+    <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2816,12 +2856,12 @@
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Added clarifying messages to Status constants in Config.xlsx
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\P3\uipath-automation-1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FEF7499-147E-4760-BCBE-BCB094D5FEF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C120F2A-ECBD-4A36-8582-9A48003D27D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -194,6 +194,15 @@
   </si>
   <si>
     <t>Status_Failure</t>
+  </si>
+  <si>
+    <t>Status message for TransactionData to record successful transaction.</t>
+  </si>
+  <si>
+    <t>Status message for TransactionData to record failed transaction.</t>
+  </si>
+  <si>
+    <t>Status message for TransactionData to record pending transaction.</t>
   </si>
 </sst>
 </file>
@@ -1695,7 +1704,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C15" sqref="A13:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1828,6 +1837,9 @@
       <c r="B13" t="s">
         <v>41</v>
       </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
@@ -1836,6 +1848,9 @@
       <c r="B14" t="s">
         <v>42</v>
       </c>
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
@@ -1843,6 +1858,9 @@
       </c>
       <c r="B15" t="s">
         <v>54</v>
+      </c>
+      <c r="C15" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
changed the config file gsuitecrential, changed the argument to match it in the process file, and updated the killall processes file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\P3\uipath-automation-1\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ohhey\Desktop\Revature_Workspace\uipath-automation-1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C120F2A-ECBD-4A36-8582-9A48003D27D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E850EE5E-CF22-488B-B34D-4CEE56CE0875}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="62835" yWindow="3420" windowWidth="17280" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -136,9 +136,6 @@
     <t>*FOR TESTING ONLY* Failed sign in credentials</t>
   </si>
   <si>
-    <t>GSuiteCredential</t>
-  </si>
-  <si>
     <t>Credential used to sign into the Gsuite Application Scope</t>
   </si>
   <si>
@@ -203,6 +200,9 @@
   </si>
   <si>
     <t>Status message for TransactionData to record pending transaction.</t>
+  </si>
+  <si>
+    <t>GSuiteOAuthCredential</t>
   </si>
 </sst>
 </file>
@@ -580,16 +580,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5234375" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.41796875" customWidth="1"/>
+    <col min="4" max="26" width="8.68359375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -676,36 +676,36 @@
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
         <v>43</v>
-      </c>
-      <c r="B10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" t="s">
         <v>36</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
         <v>38</v>
-      </c>
-      <c r="B13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1703,16 +1703,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C15" sqref="A13:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.41796875" customWidth="1"/>
+    <col min="4" max="26" width="8.68359375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1832,64 +1832,64 @@
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
         <v>40</v>
       </c>
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" t="s">
         <v>53</v>
       </c>
-      <c r="B15" t="s">
-        <v>54</v>
-      </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
         <v>46</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>47</v>
-      </c>
-      <c r="C17" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2874,12 +2874,12 @@
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.89453125" customWidth="1"/>
+    <col min="2" max="2" width="30.1015625" customWidth="1"/>
+    <col min="3" max="3" width="60.3125" customWidth="1"/>
+    <col min="4" max="26" width="65.41796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Added unattended dispatcher sequence
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\P3\uipath-automation-1\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\201019-UTA0UiPath\uipath-automation-1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C120F2A-ECBD-4A36-8582-9A48003D27D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7797030E-50BF-4E5B-91AD-F244B08C287A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4305" yWindow="3720" windowWidth="28800" windowHeight="15420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -203,6 +203,12 @@
   </si>
   <si>
     <t>Status message for TransactionData to record pending transaction.</t>
+  </si>
+  <si>
+    <t>\Documents\RevatureAutomationFiles\IntroEmailInput.txt</t>
+  </si>
+  <si>
+    <t>InputFileRelativePath</t>
   </si>
 </sst>
 </file>
@@ -584,12 +590,12 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -638,7 +644,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="28.8">
+    <row r="4" spans="1:26" ht="30">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1704,15 +1710,15 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C15" sqref="A13:C15"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1749,7 +1755,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1893,7 +1899,14 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2874,12 +2887,12 @@
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Updated dispatcher and accompanying files
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\201019-UTA0UiPath\uipath-automation-1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7797030E-50BF-4E5B-91AD-F244B08C287A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DB2BCA-8C8B-441F-A3F4-AD677DE38D77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4305" yWindow="3720" windowWidth="28800" windowHeight="15420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4305" yWindow="3720" windowWidth="28800" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -136,9 +136,6 @@
     <t>*FOR TESTING ONLY* Failed sign in credentials</t>
   </si>
   <si>
-    <t>GSuiteCredential</t>
-  </si>
-  <si>
     <t>Credential used to sign into the Gsuite Application Scope</t>
   </si>
   <si>
@@ -209,6 +206,9 @@
   </si>
   <si>
     <t>InputFileRelativePath</t>
+  </si>
+  <si>
+    <t>GSuiteOAuthCredential</t>
   </si>
 </sst>
 </file>
@@ -586,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -682,36 +682,36 @@
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
         <v>43</v>
-      </c>
-      <c r="B10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" t="s">
         <v>36</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
         <v>38</v>
-      </c>
-      <c r="B13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1709,8 +1709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1838,73 +1838,73 @@
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
         <v>40</v>
       </c>
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" t="s">
         <v>53</v>
       </c>
-      <c r="B15" t="s">
-        <v>54</v>
-      </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
         <v>46</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>47</v>
-      </c>
-      <c r="C17" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Fixed output of persisted JSON to be used in other process
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\201019-UTA0UiPath\uipath-automation-1\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\P3\uipath-automation-1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DB2BCA-8C8B-441F-A3F4-AD677DE38D77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B186C3-A98B-41F8-9137-42102CE8C0E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4305" yWindow="3720" windowWidth="28800" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t>logF_BusinessProcessName</t>
   </si>
   <si>
-    <t>Framework</t>
-  </si>
-  <si>
     <t>ProcessABCQueue</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -209,6 +206,9 @@
   </si>
   <si>
     <t>GSuiteOAuthCredential</t>
+  </si>
+  <si>
+    <t>IntroEmailsProcess</t>
   </si>
 </sst>
 </file>
@@ -587,15 +587,15 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -634,84 +634,84 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="30">
+    <row r="4" spans="1:26" ht="28.8">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
         <v>32</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
         <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
         <v>42</v>
-      </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
         <v>37</v>
-      </c>
-      <c r="B13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1713,12 +1713,12 @@
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1755,7 +1755,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1787,7 +1787,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1809,7 +1809,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -1820,7 +1820,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1831,80 +1831,80 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
         <v>39</v>
       </c>
-      <c r="B13" t="s">
-        <v>40</v>
-      </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
         <v>52</v>
       </c>
-      <c r="B15" t="s">
-        <v>53</v>
-      </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
         <v>45</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>46</v>
-      </c>
-      <c r="C17" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2887,12 +2887,12 @@
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2903,7 +2903,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Modified process name in config file to clarify output folder name
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\P3\uipath-automation-1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B186C3-A98B-41F8-9137-42102CE8C0E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510AF223-3B02-4E66-84B7-A46C8FEC8121}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -208,7 +208,7 @@
     <t>GSuiteOAuthCredential</t>
   </si>
   <si>
-    <t>IntroEmailsProcess</t>
+    <t>IntroEmails</t>
   </si>
 </sst>
 </file>
@@ -587,7 +587,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Changed filepath and config file for input file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\P3\uipath-automation-1\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\201019-UTA0UiPath\uipath-automation-1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510AF223-3B02-4E66-84B7-A46C8FEC8121}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7DD883-4579-4A1A-8FE2-DE20E094F8F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3975" yWindow="5580" windowWidth="28800" windowHeight="15420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -199,9 +199,6 @@
     <t>Status message for TransactionData to record pending transaction.</t>
   </si>
   <si>
-    <t>\Documents\RevatureAutomationFiles\IntroEmailInput.txt</t>
-  </si>
-  <si>
     <t>InputFileRelativePath</t>
   </si>
   <si>
@@ -209,6 +206,21 @@
   </si>
   <si>
     <t>IntroEmails</t>
+  </si>
+  <si>
+    <t>\RevatureAutomationFiles\</t>
+  </si>
+  <si>
+    <t>The filepath used to get the input data from the user's account. This string gets added to C:\Users\&lt;UserName&gt;</t>
+  </si>
+  <si>
+    <t>FileName</t>
+  </si>
+  <si>
+    <t>The name of the file created when filling out the form in the GetForm component</t>
+  </si>
+  <si>
+    <t>IntroEmailInput.txt</t>
   </si>
 </sst>
 </file>
@@ -586,16 +598,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -644,12 +656,12 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="28.8">
+    <row r="4" spans="1:26" ht="30">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>23</v>
@@ -694,10 +706,10 @@
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
         <v>35</v>
@@ -1709,16 +1721,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1755,7 +1767,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1901,13 +1913,26 @@
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>60</v>
+      </c>
+      <c r="C22" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" t="s">
+        <v>63</v>
+      </c>
+    </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2887,12 +2912,12 @@
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>